<commit_message>
TST: add missing test Excel file formats, rename test to test1 for clarity
</commit_message>
<xml_diff>
--- a/pandas/io/tests/data/test2.xlsx
+++ b/pandas/io/tests/data/test2.xlsx
@@ -1,36 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6d5ff33519239ae/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15780" yWindow="2240" windowWidth="12000" windowHeight="6460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Test</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>Test1</t>
   </si>
   <si>
-    <t>apple</t>
+    <t>aaaa</t>
   </si>
   <si>
-    <t>rabbit</t>
+    <t>bbbbb</t>
   </si>
 </sst>
 </file>
@@ -39,7 +44,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -73,7 +78,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -88,39 +101,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -155,7 +168,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -199,250 +212,172 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>